<commit_message>
api report gen : adding to menu
</commit_message>
<xml_diff>
--- a/Test documents/amazon scheduled report/24.xlsx
+++ b/Test documents/amazon scheduled report/24.xlsx
@@ -496,17 +496,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>402-7761907-9018739</t>
+          <t>408-7470107-3753964</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-11-22T21:07:55+00:00</t>
+          <t>2024-11-22T16:08:05+00:00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-11-22T21:21:15+00:00</t>
+          <t>2024-11-22T16:22:54+00:00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>KAR Mark Kudampuli Dried Lehyam (500 Gm)</t>
+          <t>KAR MARK kudampuli lehyam 1KG</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -528,16 +528,16 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>640</v>
+        <v>1230</v>
       </c>
       <c r="J2" t="n">
-        <v>68.58</v>
+        <v>131.79</v>
       </c>
       <c r="K2" t="n">
         <v>80</v>
       </c>
       <c r="L2" t="n">
-        <v>8.58</v>
+        <v>8.57</v>
       </c>
     </row>
     <row r="3">
@@ -546,17 +546,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>408-3619872-6041103</t>
+          <t>407-3594126-7517156</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-11-22T20:33:18+00:00</t>
+          <t>2024-11-22T15:28:15+00:00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-11-23T15:10:37+00:00</t>
+          <t>2024-11-22T18:18:58+00:00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>KAR Mark Kudampuli Dried Lehyam (500 Gm)</t>
+          <t>KAR MARK kudampuli lehyam 1KG</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -578,10 +578,10 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>640</v>
+        <v>1230</v>
       </c>
       <c r="J3" t="n">
-        <v>68.58</v>
+        <v>131.78</v>
       </c>
       <c r="K3" t="n">
         <v>80</v>
@@ -596,17 +596,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>407-5062014-7214742</t>
+          <t>406-9842547-5707502</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-11-22T17:51:42+00:00</t>
+          <t>2024-11-22T14:02:57+00:00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-11-22T18:07:04+00:00</t>
+          <t>2024-11-22T14:18:00+00:00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>KAR Mark Kudampuli Dried Lehyam (500 Gm)</t>
+          <t>KAR MARK kudampuli lehyam 1KG</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -628,10 +628,10 @@
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>640</v>
+        <v>1230</v>
       </c>
       <c r="J4" t="n">
-        <v>68.58</v>
+        <v>131.78</v>
       </c>
       <c r="K4" t="n">
         <v>80</v>
@@ -646,17 +646,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>408-7470107-3753964</t>
+          <t>406-5202604-5197163</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-11-22T16:08:05+00:00</t>
+          <t>2024-11-22T10:44:10+00:00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-11-22T16:22:54+00:00</t>
+          <t>2024-11-22T15:03:38+00:00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -681,13 +681,13 @@
         <v>1230</v>
       </c>
       <c r="J5" t="n">
-        <v>131.79</v>
+        <v>131.78</v>
       </c>
       <c r="K5" t="n">
         <v>80</v>
       </c>
       <c r="L5" t="n">
-        <v>8.57</v>
+        <v>8.58</v>
       </c>
     </row>
     <row r="6">
@@ -696,17 +696,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>405-2890357-6694768</t>
+          <t>407-0749928-3148341</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-11-22T15:55:43+00:00</t>
+          <t>2024-11-22T09:15:16+00:00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-11-22T16:10:50+00:00</t>
+          <t>2024-11-22T09:30:28+00:00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>KAR Mark Kudampuli Dried Lehyam (500 Gm)</t>
+          <t>KAR MARK kudampuli lehyam 1KG</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -728,16 +728,16 @@
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>640</v>
+        <v>1230</v>
       </c>
       <c r="J6" t="n">
-        <v>68.58</v>
+        <v>131.79</v>
       </c>
       <c r="K6" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="L6" t="n">
-        <v>8.58</v>
+        <v>4.29</v>
       </c>
     </row>
     <row r="7">
@@ -746,17 +746,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>407-3594126-7517156</t>
+          <t>171-2860293-4573126</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-11-22T15:28:15+00:00</t>
+          <t>2024-11-22T07:08:41+00:00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-11-22T18:18:58+00:00</t>
+          <t>2024-11-22T07:23:47+00:00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -796,17 +796,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>406-9842547-5707502</t>
+          <t>402-7761907-9018739</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-11-22T14:02:57+00:00</t>
+          <t>2024-11-22T21:07:55+00:00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-11-22T14:18:00+00:00</t>
+          <t>2024-11-22T21:21:15+00:00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>KAR MARK kudampuli lehyam 1KG</t>
+          <t>KAR Mark Kudampuli Dried Lehyam (500 Gm)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -828,10 +828,10 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>1230</v>
+        <v>640</v>
       </c>
       <c r="J8" t="n">
-        <v>131.78</v>
+        <v>68.58</v>
       </c>
       <c r="K8" t="n">
         <v>80</v>
@@ -846,17 +846,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>408-2937479-4182750</t>
+          <t>408-3619872-6041103</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024-11-22T13:05:03+00:00</t>
+          <t>2024-11-22T20:33:18+00:00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-11-22T13:20:13+00:00</t>
+          <t>2024-11-23T15:10:37+00:00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -881,13 +881,13 @@
         <v>640</v>
       </c>
       <c r="J9" t="n">
-        <v>68.56999999999999</v>
+        <v>68.58</v>
       </c>
       <c r="K9" t="n">
         <v>80</v>
       </c>
       <c r="L9" t="n">
-        <v>8.57</v>
+        <v>8.58</v>
       </c>
     </row>
     <row r="10">
@@ -896,17 +896,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>406-5202604-5197163</t>
+          <t>407-5062014-7214742</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024-11-22T10:44:10+00:00</t>
+          <t>2024-11-22T17:51:42+00:00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-11-22T15:03:38+00:00</t>
+          <t>2024-11-22T18:07:04+00:00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>KAR MARK kudampuli lehyam 1KG</t>
+          <t>KAR Mark Kudampuli Dried Lehyam (500 Gm)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -928,10 +928,10 @@
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>1230</v>
+        <v>640</v>
       </c>
       <c r="J10" t="n">
-        <v>131.78</v>
+        <v>68.58</v>
       </c>
       <c r="K10" t="n">
         <v>80</v>
@@ -946,17 +946,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>407-6478206-4772334</t>
+          <t>405-2890357-6694768</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2024-11-22T09:54:02+00:00</t>
+          <t>2024-11-22T15:55:43+00:00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-11-22T10:03:29+00:00</t>
+          <t>2024-11-22T16:10:50+00:00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -996,17 +996,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>171-7906369-9845952</t>
+          <t>408-2937479-4182750</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2024-11-22T09:32:17+00:00</t>
+          <t>2024-11-22T13:05:03+00:00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-11-22T09:41:33+00:00</t>
+          <t>2024-11-22T13:20:13+00:00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1031,13 +1031,13 @@
         <v>640</v>
       </c>
       <c r="J12" t="n">
-        <v>68.58</v>
+        <v>68.56999999999999</v>
       </c>
       <c r="K12" t="n">
         <v>80</v>
       </c>
       <c r="L12" t="n">
-        <v>8.58</v>
+        <v>8.57</v>
       </c>
     </row>
     <row r="13">
@@ -1046,17 +1046,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>407-0749928-3148341</t>
+          <t>407-6478206-4772334</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2024-11-22T09:15:16+00:00</t>
+          <t>2024-11-22T09:54:02+00:00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-11-22T09:30:28+00:00</t>
+          <t>2024-11-22T10:03:29+00:00</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1081,13 +1081,13 @@
         <v>640</v>
       </c>
       <c r="J13" t="n">
-        <v>68.56999999999999</v>
+        <v>68.58</v>
       </c>
       <c r="K13" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="L13" t="n">
-        <v>4.29</v>
+        <v>8.58</v>
       </c>
     </row>
     <row r="14">
@@ -1096,17 +1096,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>407-0749928-3148341</t>
+          <t>171-7906369-9845952</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2024-11-22T09:15:16+00:00</t>
+          <t>2024-11-22T09:32:17+00:00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-11-22T09:30:28+00:00</t>
+          <t>2024-11-22T09:41:33+00:00</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>KAR MARK kudampuli lehyam 1KG</t>
+          <t>KAR Mark Kudampuli Dried Lehyam (500 Gm)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1128,16 +1128,16 @@
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>1230</v>
+        <v>640</v>
       </c>
       <c r="J14" t="n">
-        <v>131.79</v>
+        <v>68.58</v>
       </c>
       <c r="K14" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="L14" t="n">
-        <v>4.29</v>
+        <v>8.58</v>
       </c>
     </row>
     <row r="15">
@@ -1146,17 +1146,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>405-4471990-3110724</t>
+          <t>407-0749928-3148341</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2024-11-22T08:29:42+00:00</t>
+          <t>2024-11-22T09:15:16+00:00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-11-22T08:44:25+00:00</t>
+          <t>2024-11-22T09:30:28+00:00</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1181,13 +1181,13 @@
         <v>640</v>
       </c>
       <c r="J15" t="n">
-        <v>68.58</v>
+        <v>68.56999999999999</v>
       </c>
       <c r="K15" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="L15" t="n">
-        <v>8.58</v>
+        <v>4.29</v>
       </c>
     </row>
     <row r="16">
@@ -1196,17 +1196,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>405-5684197-8263504</t>
+          <t>405-4471990-3110724</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2024-11-22T08:15:07+00:00</t>
+          <t>2024-11-22T08:29:42+00:00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-11-22T08:30:16+00:00</t>
+          <t>2024-11-22T08:44:25+00:00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1246,17 +1246,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>405-5142500-8749156</t>
+          <t>405-5684197-8263504</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2024-11-22T07:26:12+00:00</t>
+          <t>2024-11-22T08:15:07+00:00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-11-22T07:43:38+00:00</t>
+          <t>2024-11-22T08:30:16+00:00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1266,7 +1266,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>KAR Mark Kudampuli Dried Lehyam For Weight Loss And Reduce Belly Fat(750 Gm)</t>
+          <t>KAR Mark Kudampuli Dried Lehyam (500 Gm)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1278,10 +1278,10 @@
         <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>950</v>
+        <v>640</v>
       </c>
       <c r="J17" t="n">
-        <v>101.78</v>
+        <v>68.58</v>
       </c>
       <c r="K17" t="n">
         <v>80</v>
@@ -1296,17 +1296,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>171-2860293-4573126</t>
+          <t>405-5142500-8749156</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2024-11-22T07:08:41+00:00</t>
+          <t>2024-11-22T07:26:12+00:00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-11-22T07:23:47+00:00</t>
+          <t>2024-11-22T07:43:38+00:00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>KAR MARK kudampuli lehyam 1KG</t>
+          <t>KAR Mark Kudampuli Dried Lehyam For Weight Loss And Reduce Belly Fat(750 Gm)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1328,10 +1328,10 @@
         <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>1230</v>
+        <v>950</v>
       </c>
       <c r="J18" t="n">
-        <v>131.78</v>
+        <v>101.78</v>
       </c>
       <c r="K18" t="n">
         <v>80</v>

</xml_diff>